<commit_message>
update leave card 1/9/2024 4:42 pm
</commit_message>
<xml_diff>
--- a/CASUAL/LA CENRO CITY HALL BASED/BAY, AMIE.xlsx
+++ b/CASUAL/LA CENRO CITY HALL BASED/BAY, AMIE.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dole-pc\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA CENRO CITY HALL BASED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA CENRO CITY HALL BASED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6878582-9ECA-4348-B737-DAA8089246D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -28,7 +27,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="101">
   <si>
     <t>PERIOD</t>
   </si>
@@ -338,12 +337,15 @@
   </si>
   <si>
     <t>11/21,24,28/2023</t>
+  </si>
+  <si>
+    <t>01/16-19/2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -725,17 +727,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -745,6 +744,9 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1275,7 +1277,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1318,7 +1320,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1382,7 +1384,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1442,7 +1444,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1508,7 +1510,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1571,7 +1573,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1669,7 +1671,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1728,7 +1730,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1793,7 +1795,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1836,7 +1838,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1911,7 +1913,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2097,7 +2099,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2163,7 +2165,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2221,7 +2223,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2287,7 +2289,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2343,7 +2345,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2418,7 +2420,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2461,7 +2463,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2527,7 +2529,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2583,7 +2585,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2662,7 +2664,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -2679,25 +2681,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:K142" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K142" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="21">
+    <tableColumn id="1" name="PERIOD" dataDxfId="25"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="24"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="23"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="22"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="21">
       <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="19">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="20"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="17">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="17">
       <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="15"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2709,25 +2711,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A8:K72" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K72" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3034,7 +3036,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -3044,7 +3046,7 @@
       <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3052,34 +3054,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3696" topLeftCell="A71" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A86" activePane="bottomLeft"/>
       <selection activeCell="E10" sqref="E10"/>
-      <selection pane="bottomLeft" activeCell="E76" sqref="E76"/>
+      <selection pane="bottomLeft" activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -3091,16 +3093,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="53"/>
+      <c r="K2" s="54"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -3109,18 +3111,18 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="56">
+      <c r="F3" s="55">
         <v>42020</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="53"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="58"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -3131,18 +3133,18 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="53"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="53"/>
+      <c r="K4" s="54"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -3150,7 +3152,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -3163,24 +3165,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54" t="s">
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -3215,7 +3217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -3224,7 +3226,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])</f>
-        <v>39.415999999999997</v>
+        <v>32.915999999999997</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -3234,12 +3236,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])</f>
-        <v>87.5</v>
+        <v>90</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>44</v>
       </c>
@@ -3261,7 +3263,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>43101</v>
       </c>
@@ -3281,7 +3283,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>43132</v>
       </c>
@@ -3301,7 +3303,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="49"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>43160</v>
       </c>
@@ -3327,7 +3329,7 @@
         <v>43185</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>43191</v>
       </c>
@@ -3347,7 +3349,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="49"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>43221</v>
       </c>
@@ -3367,7 +3369,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="49"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="40">
         <v>43252</v>
       </c>
@@ -3387,7 +3389,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="50"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="40">
         <v>43282</v>
       </c>
@@ -3407,7 +3409,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
         <v>43313</v>
       </c>
@@ -3427,7 +3429,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="40">
         <v>43344</v>
       </c>
@@ -3447,7 +3449,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="40">
         <v>43374</v>
       </c>
@@ -3467,7 +3469,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="40">
         <v>43405</v>
       </c>
@@ -3487,7 +3489,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="40">
         <v>43435</v>
       </c>
@@ -3513,7 +3515,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
         <v>51</v>
       </c>
@@ -3531,7 +3533,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="40">
         <v>43466</v>
       </c>
@@ -3551,7 +3553,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="40">
         <v>43497</v>
       </c>
@@ -3571,7 +3573,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="40">
         <v>43525</v>
       </c>
@@ -3591,7 +3593,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="40">
         <v>43556</v>
       </c>
@@ -3611,7 +3613,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="40">
         <v>43586</v>
       </c>
@@ -3631,7 +3633,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="40">
         <v>43617</v>
       </c>
@@ -3651,7 +3653,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="40">
         <v>43647</v>
       </c>
@@ -3671,7 +3673,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="40">
         <v>43678</v>
       </c>
@@ -3691,7 +3693,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="40">
         <v>43709</v>
       </c>
@@ -3711,7 +3713,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="40">
         <v>43739</v>
       </c>
@@ -3731,7 +3733,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="40">
         <v>43770</v>
       </c>
@@ -3751,7 +3753,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="40">
         <v>43800</v>
       </c>
@@ -3775,7 +3777,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
         <v>52</v>
       </c>
@@ -3793,7 +3795,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="40">
         <v>43831</v>
       </c>
@@ -3813,7 +3815,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="40">
         <v>43862</v>
       </c>
@@ -3833,7 +3835,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="40">
         <v>43891</v>
       </c>
@@ -3853,7 +3855,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="40">
         <v>43922</v>
       </c>
@@ -3873,7 +3875,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="40">
         <v>43952</v>
       </c>
@@ -3893,7 +3895,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="40">
         <v>43983</v>
       </c>
@@ -3913,7 +3915,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="40">
         <v>44013</v>
       </c>
@@ -3933,7 +3935,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="40">
         <v>44044</v>
       </c>
@@ -3953,7 +3955,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="40">
         <v>44075</v>
       </c>
@@ -3973,7 +3975,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="40">
         <v>44105</v>
       </c>
@@ -3993,7 +3995,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="40">
         <v>44136</v>
       </c>
@@ -4013,7 +4015,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="40">
         <v>44166</v>
       </c>
@@ -4037,7 +4039,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="40"/>
       <c r="B49" s="20" t="s">
         <v>54</v>
@@ -4057,7 +4059,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="48" t="s">
         <v>53</v>
       </c>
@@ -4075,7 +4077,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="40">
         <v>44197</v>
       </c>
@@ -4095,7 +4097,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="40">
         <v>44228</v>
       </c>
@@ -4115,7 +4117,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="40">
         <v>44256</v>
       </c>
@@ -4135,7 +4137,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="40">
         <v>44287</v>
       </c>
@@ -4155,7 +4157,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="40">
         <v>44317</v>
       </c>
@@ -4175,7 +4177,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="40">
         <v>44348</v>
       </c>
@@ -4195,7 +4197,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="40">
         <v>44378</v>
       </c>
@@ -4215,7 +4217,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="40">
         <v>44409</v>
       </c>
@@ -4235,7 +4237,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="40">
         <v>44440</v>
       </c>
@@ -4255,7 +4257,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="40">
         <v>44470</v>
       </c>
@@ -4275,7 +4277,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="40">
         <v>44501</v>
       </c>
@@ -4295,7 +4297,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="40">
         <v>44531</v>
       </c>
@@ -4319,7 +4321,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="48" t="s">
         <v>56</v>
       </c>
@@ -4337,7 +4339,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="40">
         <v>44562</v>
       </c>
@@ -4357,7 +4359,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="40">
         <v>44593</v>
       </c>
@@ -4377,7 +4379,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="40">
         <v>44621</v>
       </c>
@@ -4403,7 +4405,7 @@
         <v>44631</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="40"/>
       <c r="B67" s="20" t="s">
         <v>92</v>
@@ -4423,7 +4425,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="49"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="40">
         <v>44652</v>
       </c>
@@ -4449,7 +4451,7 @@
         <v>44677</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="40"/>
       <c r="B69" s="20" t="s">
         <v>78</v>
@@ -4469,7 +4471,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="49"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="40">
         <v>44682</v>
       </c>
@@ -4495,7 +4497,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="40"/>
       <c r="B71" s="20" t="s">
         <v>91</v>
@@ -4515,7 +4517,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="40">
         <v>44713</v>
       </c>
@@ -4541,7 +4543,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="40"/>
       <c r="B73" s="20" t="s">
         <v>89</v>
@@ -4561,7 +4563,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="40">
         <v>44743</v>
       </c>
@@ -4587,7 +4589,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="40"/>
       <c r="B75" s="20" t="s">
         <v>87</v>
@@ -4607,7 +4609,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="40">
         <v>44774</v>
       </c>
@@ -4633,7 +4635,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="40"/>
       <c r="B77" s="20" t="s">
         <v>84</v>
@@ -4653,7 +4655,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="40">
         <v>44805</v>
       </c>
@@ -4679,7 +4681,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="40"/>
       <c r="B79" s="20" t="s">
         <v>81</v>
@@ -4699,7 +4701,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="40">
         <v>44835</v>
       </c>
@@ -4725,7 +4727,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="40"/>
       <c r="B81" s="20" t="s">
         <v>78</v>
@@ -4745,7 +4747,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="40">
         <v>44866</v>
       </c>
@@ -4765,7 +4767,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="40">
         <v>44896</v>
       </c>
@@ -4789,7 +4791,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="40"/>
       <c r="B84" s="20" t="s">
         <v>74</v>
@@ -4811,7 +4813,7 @@
         <v>44907</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="40"/>
       <c r="B85" s="20" t="s">
         <v>75</v>
@@ -4831,7 +4833,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="49"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="48" t="s">
         <v>61</v>
       </c>
@@ -4849,7 +4851,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="40">
         <v>44957</v>
       </c>
@@ -4869,7 +4871,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="40">
         <v>44985</v>
       </c>
@@ -4889,7 +4891,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="40">
         <v>45016</v>
       </c>
@@ -4909,7 +4911,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="40">
         <v>45046</v>
       </c>
@@ -4929,7 +4931,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="40">
         <v>45077</v>
       </c>
@@ -4949,7 +4951,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="40">
         <v>45107</v>
       </c>
@@ -4969,7 +4971,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="40">
         <v>45138</v>
       </c>
@@ -4989,7 +4991,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="40">
         <v>45169</v>
       </c>
@@ -5009,7 +5011,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="40">
         <v>45199</v>
       </c>
@@ -5029,7 +5031,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="40">
         <v>45230</v>
       </c>
@@ -5049,43 +5051,51 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="40">
         <v>45260</v>
       </c>
       <c r="B97" s="20"/>
-      <c r="C97" s="13"/>
+      <c r="C97" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D97" s="39"/>
       <c r="E97" s="9"/>
       <c r="F97" s="20"/>
-      <c r="G97" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G97" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H97" s="39"/>
       <c r="I97" s="9"/>
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="40">
         <v>45291</v>
       </c>
-      <c r="B98" s="20"/>
-      <c r="C98" s="13"/>
-      <c r="D98" s="39"/>
+      <c r="B98" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C98" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D98" s="39">
+        <v>5</v>
+      </c>
       <c r="E98" s="9"/>
       <c r="F98" s="20"/>
-      <c r="G98" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G98" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H98" s="39"/>
       <c r="I98" s="9"/>
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="48" t="s">
         <v>96</v>
       </c>
@@ -5103,13 +5113,17 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="40">
         <v>45322</v>
       </c>
-      <c r="B100" s="20"/>
+      <c r="B100" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="C100" s="13"/>
-      <c r="D100" s="39"/>
+      <c r="D100" s="39">
+        <v>4</v>
+      </c>
       <c r="E100" s="9"/>
       <c r="F100" s="20"/>
       <c r="G100" s="13" t="str">
@@ -5119,9 +5133,11 @@
       <c r="H100" s="39"/>
       <c r="I100" s="9"/>
       <c r="J100" s="11"/>
-      <c r="K100" s="20"/>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K100" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="40">
         <v>45351</v>
       </c>
@@ -5139,7 +5155,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="40">
         <v>45382</v>
       </c>
@@ -5157,7 +5173,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="40">
         <v>45412</v>
       </c>
@@ -5175,7 +5191,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="40">
         <v>45443</v>
       </c>
@@ -5193,7 +5209,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="40">
         <v>45473</v>
       </c>
@@ -5211,7 +5227,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="40">
         <v>45504</v>
       </c>
@@ -5229,7 +5245,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="40">
         <v>45535</v>
       </c>
@@ -5247,7 +5263,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="40">
         <v>45565</v>
       </c>
@@ -5265,7 +5281,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="40">
         <v>45596</v>
       </c>
@@ -5283,7 +5299,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="40">
         <v>45626</v>
       </c>
@@ -5301,7 +5317,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="40">
         <v>45657</v>
       </c>
@@ -5319,7 +5335,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -5335,7 +5351,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -5351,7 +5367,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -5367,7 +5383,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -5383,7 +5399,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -5399,7 +5415,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -5415,7 +5431,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -5431,7 +5447,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -5447,7 +5463,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -5463,7 +5479,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -5479,7 +5495,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -5495,7 +5511,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -5511,7 +5527,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -5527,7 +5543,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -5543,7 +5559,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -5559,7 +5575,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -5575,7 +5591,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -5591,7 +5607,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -5607,7 +5623,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="40"/>
       <c r="B130" s="20"/>
       <c r="C130" s="13"/>
@@ -5623,7 +5639,7 @@
       <c r="J130" s="11"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="40"/>
       <c r="B131" s="20"/>
       <c r="C131" s="13"/>
@@ -5639,7 +5655,7 @@
       <c r="J131" s="11"/>
       <c r="K131" s="20"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="40"/>
       <c r="B132" s="20"/>
       <c r="C132" s="13"/>
@@ -5655,7 +5671,7 @@
       <c r="J132" s="11"/>
       <c r="K132" s="20"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="40"/>
       <c r="B133" s="20"/>
       <c r="C133" s="13"/>
@@ -5671,7 +5687,7 @@
       <c r="J133" s="11"/>
       <c r="K133" s="20"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="40"/>
       <c r="B134" s="20"/>
       <c r="C134" s="13"/>
@@ -5687,7 +5703,7 @@
       <c r="J134" s="11"/>
       <c r="K134" s="20"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="40"/>
       <c r="B135" s="20"/>
       <c r="C135" s="13"/>
@@ -5703,7 +5719,7 @@
       <c r="J135" s="11"/>
       <c r="K135" s="20"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="40"/>
       <c r="B136" s="20"/>
       <c r="C136" s="13"/>
@@ -5719,7 +5735,7 @@
       <c r="J136" s="11"/>
       <c r="K136" s="20"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="40"/>
       <c r="B137" s="20"/>
       <c r="C137" s="13"/>
@@ -5735,7 +5751,7 @@
       <c r="J137" s="11"/>
       <c r="K137" s="20"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="40"/>
       <c r="B138" s="20"/>
       <c r="C138" s="13"/>
@@ -5751,7 +5767,7 @@
       <c r="J138" s="11"/>
       <c r="K138" s="20"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="40"/>
       <c r="B139" s="20"/>
       <c r="C139" s="13"/>
@@ -5767,7 +5783,7 @@
       <c r="J139" s="11"/>
       <c r="K139" s="20"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="40"/>
       <c r="B140" s="20"/>
       <c r="C140" s="13"/>
@@ -5783,7 +5799,7 @@
       <c r="J140" s="11"/>
       <c r="K140" s="20"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="40"/>
       <c r="B141" s="20"/>
       <c r="C141" s="13"/>
@@ -5799,7 +5815,7 @@
       <c r="J141" s="11"/>
       <c r="K141" s="20"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="41"/>
       <c r="B142" s="15"/>
       <c r="C142" s="42"/>
@@ -5817,23 +5833,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5856,34 +5872,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K72"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3696" topLeftCell="A17" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A17" activePane="bottomLeft"/>
       <selection activeCell="B3" sqref="B3:C3"/>
       <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -5895,16 +5911,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="53"/>
+      <c r="K2" s="54"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -5913,16 +5929,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="52"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="53"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="58"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -5933,18 +5949,18 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="53"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="53"/>
+      <c r="K4" s="54"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -5952,7 +5968,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -5965,24 +5981,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54" t="s">
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -6017,7 +6033,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -6041,7 +6057,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>44</v>
       </c>
@@ -6063,7 +6079,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>43132</v>
       </c>
@@ -6087,7 +6103,7 @@
         <v>43152</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>43191</v>
       </c>
@@ -6109,7 +6125,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
         <v>56</v>
       </c>
@@ -6127,7 +6143,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>44593</v>
       </c>
@@ -6149,7 +6165,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>44621</v>
       </c>
@@ -6173,7 +6189,7 @@
         <v>44631</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="40">
         <v>44835</v>
       </c>
@@ -6197,7 +6213,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
         <v>61</v>
       </c>
@@ -6215,7 +6231,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
         <v>44927</v>
       </c>
@@ -6239,7 +6255,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="40">
         <v>45047</v>
       </c>
@@ -6263,7 +6279,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="20" t="s">
         <v>66</v>
@@ -6285,7 +6301,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="20" t="s">
         <v>68</v>
@@ -6307,7 +6323,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="40">
         <v>45103</v>
       </c>
@@ -6331,7 +6347,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="40">
         <v>45111</v>
       </c>
@@ -6355,7 +6371,7 @@
         <v>45110</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="40">
         <v>45133</v>
       </c>
@@ -6379,7 +6395,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="40">
         <v>45170</v>
       </c>
@@ -6403,7 +6419,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="40">
         <v>45200</v>
       </c>
@@ -6427,7 +6443,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="40">
         <v>45231</v>
       </c>
@@ -6451,7 +6467,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="40"/>
       <c r="B28" s="20" t="s">
         <v>97</v>
@@ -6473,7 +6489,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="40">
         <v>45245</v>
       </c>
@@ -6497,7 +6513,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="40"/>
       <c r="B30" s="20"/>
       <c r="C30" s="13"/>
@@ -6513,7 +6529,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="40"/>
       <c r="B31" s="20"/>
       <c r="C31" s="13"/>
@@ -6529,7 +6545,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="40"/>
       <c r="B32" s="20"/>
       <c r="C32" s="13"/>
@@ -6545,7 +6561,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="40"/>
       <c r="B33" s="20"/>
       <c r="C33" s="13"/>
@@ -6561,7 +6577,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="40"/>
       <c r="B34" s="20"/>
       <c r="C34" s="13"/>
@@ -6577,7 +6593,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="40"/>
       <c r="B35" s="20"/>
       <c r="C35" s="13"/>
@@ -6593,7 +6609,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="40"/>
       <c r="B36" s="20"/>
       <c r="C36" s="13"/>
@@ -6609,7 +6625,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="40"/>
       <c r="B37" s="20"/>
       <c r="C37" s="13"/>
@@ -6625,7 +6641,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="40"/>
       <c r="B38" s="20"/>
       <c r="C38" s="13"/>
@@ -6641,7 +6657,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="40"/>
       <c r="B39" s="20"/>
       <c r="C39" s="13"/>
@@ -6657,7 +6673,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="40"/>
       <c r="B40" s="20"/>
       <c r="C40" s="13"/>
@@ -6673,7 +6689,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="40"/>
       <c r="B41" s="20"/>
       <c r="C41" s="13"/>
@@ -6689,7 +6705,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="40"/>
       <c r="B42" s="20"/>
       <c r="C42" s="13"/>
@@ -6705,7 +6721,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="40"/>
       <c r="B43" s="20"/>
       <c r="C43" s="13"/>
@@ -6721,7 +6737,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="40"/>
       <c r="B44" s="20"/>
       <c r="C44" s="13"/>
@@ -6737,7 +6753,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="40"/>
       <c r="B45" s="20"/>
       <c r="C45" s="13"/>
@@ -6753,7 +6769,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="40"/>
       <c r="B46" s="20"/>
       <c r="C46" s="13"/>
@@ -6769,7 +6785,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="40"/>
       <c r="B47" s="20"/>
       <c r="C47" s="13"/>
@@ -6785,7 +6801,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="40"/>
       <c r="B48" s="20"/>
       <c r="C48" s="13"/>
@@ -6801,7 +6817,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="40"/>
       <c r="B49" s="20"/>
       <c r="C49" s="13"/>
@@ -6817,7 +6833,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="40"/>
       <c r="B50" s="20"/>
       <c r="C50" s="13"/>
@@ -6833,7 +6849,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="40"/>
       <c r="B51" s="20"/>
       <c r="C51" s="13"/>
@@ -6849,7 +6865,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="40"/>
       <c r="B52" s="20"/>
       <c r="C52" s="13"/>
@@ -6865,7 +6881,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="40"/>
       <c r="B53" s="20"/>
       <c r="C53" s="13"/>
@@ -6881,7 +6897,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="40"/>
       <c r="B54" s="20"/>
       <c r="C54" s="13"/>
@@ -6897,7 +6913,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="40"/>
       <c r="B55" s="20"/>
       <c r="C55" s="13"/>
@@ -6913,7 +6929,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="40"/>
       <c r="B56" s="20"/>
       <c r="C56" s="13"/>
@@ -6929,7 +6945,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="40"/>
       <c r="B57" s="20"/>
       <c r="C57" s="13"/>
@@ -6945,7 +6961,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="40"/>
       <c r="B58" s="20"/>
       <c r="C58" s="13"/>
@@ -6961,7 +6977,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="40"/>
       <c r="B59" s="20"/>
       <c r="C59" s="13"/>
@@ -6977,7 +6993,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="40"/>
       <c r="B60" s="20"/>
       <c r="C60" s="13"/>
@@ -6993,7 +7009,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="40"/>
       <c r="B61" s="20"/>
       <c r="C61" s="13"/>
@@ -7009,7 +7025,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="40"/>
       <c r="B62" s="20"/>
       <c r="C62" s="13"/>
@@ -7025,7 +7041,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="40"/>
       <c r="B63" s="20"/>
       <c r="C63" s="13"/>
@@ -7041,7 +7057,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="40"/>
       <c r="B64" s="20"/>
       <c r="C64" s="13"/>
@@ -7057,7 +7073,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="40"/>
       <c r="B65" s="20"/>
       <c r="C65" s="13"/>
@@ -7073,7 +7089,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="40"/>
       <c r="B66" s="20"/>
       <c r="C66" s="13"/>
@@ -7089,7 +7105,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="40"/>
       <c r="B67" s="20"/>
       <c r="C67" s="13"/>
@@ -7105,7 +7121,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="40"/>
       <c r="B68" s="20"/>
       <c r="C68" s="13"/>
@@ -7121,7 +7137,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="40"/>
       <c r="B69" s="20"/>
       <c r="C69" s="13"/>
@@ -7137,7 +7153,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="40"/>
       <c r="B70" s="20"/>
       <c r="C70" s="13"/>
@@ -7153,7 +7169,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="40"/>
       <c r="B71" s="20"/>
       <c r="C71" s="13"/>
@@ -7169,7 +7185,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="41"/>
       <c r="B72" s="15"/>
       <c r="C72" s="42"/>
@@ -7200,10 +7216,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7226,28 +7242,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="59" t="s">
         <v>33</v>
       </c>
@@ -7260,7 +7276,7 @@
       <c r="K1" s="60"/>
       <c r="L1" s="60"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -7289,7 +7305,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>80.906999999999996</v>
       </c>
@@ -7317,17 +7333,17 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>72</v>
       </c>
@@ -7351,10 +7367,10 @@
       <c r="K6" s="61"/>
       <c r="L6" s="61"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <f>SUM('2018 LEAVE CREDITS'!E9,'2018 LEAVE CREDITS'!I9)</f>
-        <v>126.916</v>
+        <v>122.916</v>
       </c>
       <c r="C7" s="37">
         <v>1</v>
@@ -7382,7 +7398,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -7408,7 +7424,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -7434,7 +7450,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -7460,7 +7476,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -7486,7 +7502,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -7512,7 +7528,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -7538,7 +7554,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -7564,7 +7580,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -7584,7 +7600,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -7604,7 +7620,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -7624,7 +7640,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -7645,7 +7661,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -7666,7 +7682,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -7687,7 +7703,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -7708,7 +7724,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -7729,7 +7745,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -7750,7 +7766,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -7771,7 +7787,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -7792,7 +7808,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -7813,7 +7829,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -7834,7 +7850,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -7855,7 +7871,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -7876,7 +7892,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -7897,7 +7913,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -7918,7 +7934,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -7939,7 +7955,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -7960,7 +7976,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -7981,7 +7997,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -8002,7 +8018,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -8023,7 +8039,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -8044,7 +8060,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -8053,7 +8069,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -8062,7 +8078,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -8071,7 +8087,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -8080,7 +8096,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -8089,7 +8105,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -8098,7 +8114,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -8107,7 +8123,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -8116,7 +8132,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -8125,7 +8141,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -8134,7 +8150,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -8143,7 +8159,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -8152,7 +8168,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -8161,7 +8177,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -8170,7 +8186,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -8179,7 +8195,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -8188,7 +8204,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -8197,7 +8213,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -8206,7 +8222,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -8215,7 +8231,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -8224,7 +8240,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -8233,7 +8249,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -8242,7 +8258,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -8251,7 +8267,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -8260,7 +8276,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -8269,7 +8285,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -8278,7 +8294,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -8287,7 +8303,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -8296,7 +8312,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -8305,7 +8321,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>